<commit_message>
New stepsizes -> edited stepsize 2 and 5 to absolute of gamma in the denominator instead of quadratic term
</commit_message>
<xml_diff>
--- a/Code/SampleRun_Environment_Solar/Lower_bounds.xlsx
+++ b/Code/SampleRun_Environment_Solar/Lower_bounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\A_Uni\HiWi\ArticleSubgradient\Code\SampleRun_Environment_Solar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC5E0C8-4DA0-4305-9E3C-723A3415CDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7A7B8C-8FE5-4A66-9E0F-123B471127B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="117">
   <si>
     <t>Column1</t>
   </si>
@@ -389,6 +389,15 @@
   </si>
   <si>
     <t>QP av:</t>
+  </si>
+  <si>
+    <t>IR av:</t>
+  </si>
+  <si>
+    <t>AP av:</t>
+  </si>
+  <si>
+    <t>AV IR 8:</t>
   </si>
 </sst>
 </file>
@@ -834,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -989,7 +998,8 @@
         <v>19</v>
       </c>
       <c r="E5" s="2">
-        <v>-1E-3</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N5)/N5</f>
+        <v>-8.838945932361611E-2</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>20</v>
@@ -998,8 +1008,8 @@
         <v>21</v>
       </c>
       <c r="H5" s="2">
-        <f>(Lower_bounds[[#This Row],[Column5]]-N5)/Lower_bounds[[#This Row],[Column5]]</f>
-        <v>-0.19925945061568945</v>
+        <f>(Lower_bounds[[#This Row],[Column5]]-N5)/N5</f>
+        <v>-0.16615207869605811</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>22</v>
@@ -1008,7 +1018,7 @@
         <v>23</v>
       </c>
       <c r="K5" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N5)/Lower_bounds[[#This Row],[Column7]]</f>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N5)/N5</f>
         <v>0</v>
       </c>
       <c r="M5" t="s">
@@ -1032,8 +1042,8 @@
         <v>26</v>
       </c>
       <c r="E6" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-280.05)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>-8.4792376820576332E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N6)/N6</f>
+        <v>-7.8164613461881749E-2</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
@@ -1042,8 +1052,8 @@
         <v>28</v>
       </c>
       <c r="H6" s="2">
-        <f>(Lower_bounds[[#This Row],[Column5]]-N6)/Lower_bounds[[#This Row],[Column5]]</f>
-        <v>-0.20430893609701567</v>
+        <f>(Lower_bounds[[#This Row],[Column5]]-N6)/N6</f>
+        <v>-0.16964827709337624</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>29</v>
@@ -1052,12 +1062,12 @@
         <v>30</v>
       </c>
       <c r="K6" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N6)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>-3.1881358360796182E-3</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N6)/N6</f>
+        <v>-3.1780039278699744E-3</v>
       </c>
       <c r="M6" s="3">
         <f>AVERAGE(K5:K20)</f>
-        <v>3.5656302554698344E-2</v>
+        <v>3.8674305490522649E-2</v>
       </c>
       <c r="N6">
         <v>280.05</v>
@@ -1077,8 +1087,8 @@
         <v>33</v>
       </c>
       <c r="E7" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-280.98)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>-5.9662090813093947E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N7)/N7</f>
+        <v>-5.6302939711011434E-2</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>34</v>
@@ -1087,8 +1097,8 @@
         <v>35</v>
       </c>
       <c r="H7" s="2">
-        <f>(Lower_bounds[[#This Row],[Column5]]-N7)/Lower_bounds[[#This Row],[Column5]]</f>
-        <v>-0.20701061042140997</v>
+        <f>(Lower_bounds[[#This Row],[Column5]]-N7)/N7</f>
+        <v>-0.17150686881628593</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>36</v>
@@ -1097,8 +1107,11 @@
         <v>37</v>
       </c>
       <c r="K7" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N7)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>-1.9612737581571563E-3</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N7)/N7</f>
+        <v>-1.957434692860742E-3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>114</v>
       </c>
       <c r="N7">
         <v>280.98</v>
@@ -1118,8 +1131,8 @@
         <v>40</v>
       </c>
       <c r="E8" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-283.99)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>-6.9924273819839511E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N8)/N8</f>
+        <v>-6.5354413887812962E-2</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>41</v>
@@ -1128,8 +1141,8 @@
         <v>42</v>
       </c>
       <c r="H8" s="2">
-        <f>(Lower_bounds[[#This Row],[Column5]]-N8)/Lower_bounds[[#This Row],[Column5]]</f>
-        <v>-2.4273245329293869E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column5]]-N8)/N8</f>
+        <v>-2.3698017535828789E-2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>43</v>
@@ -1138,8 +1151,12 @@
         <v>44</v>
       </c>
       <c r="K8" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N8)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>-9.8692326671611708E-4</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N8)/N8</f>
+        <v>-9.8595020951452355E-4</v>
+      </c>
+      <c r="M8" s="3">
+        <f>AVERAGE(E5:E20)</f>
+        <v>2.7668687100781734E-2</v>
       </c>
       <c r="N8">
         <v>283.99</v>
@@ -1159,8 +1176,8 @@
         <v>47</v>
       </c>
       <c r="E9" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-246.47)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>-3.3894039179495836E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N9)/N9</f>
+        <v>-3.3175163239647996E-2</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>48</v>
@@ -1178,8 +1195,11 @@
         <v>51</v>
       </c>
       <c r="K9" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N9)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>7.7665995975855408E-3</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N9)/N9</f>
+        <v>7.8273918157115898E-3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>115</v>
       </c>
       <c r="N9">
         <v>246.57</v>
@@ -1199,8 +1219,8 @@
         <v>53</v>
       </c>
       <c r="E10" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-232.13)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>3.2912552597591994E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N10)/N10</f>
+        <v>3.4032654116228002E-2</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>48</v>
@@ -1218,8 +1238,12 @@
         <v>56</v>
       </c>
       <c r="K10" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N10)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>7.8593260032548767E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N10)/N10</f>
+        <v>8.529703183560941E-2</v>
+      </c>
+      <c r="M10" s="3">
+        <f>AVERAGE(H5:H8)</f>
+        <v>-0.13275131053538727</v>
       </c>
       <c r="N10">
         <v>232.13</v>
@@ -1239,8 +1263,8 @@
         <v>58</v>
       </c>
       <c r="E11" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-232.3)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>8.7624209575429088E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N11)/N11</f>
+        <v>9.6039603960396042E-2</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>48</v>
@@ -1258,8 +1282,8 @@
         <v>61</v>
       </c>
       <c r="K11" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N11)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>7.9927122940430848E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N11)/N11</f>
+        <v>8.687042617305199E-2</v>
       </c>
       <c r="N11">
         <v>232.3</v>
@@ -1279,8 +1303,8 @@
         <v>63</v>
       </c>
       <c r="E12" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-246.98)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>4.4306001625198377E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N12)/N12</f>
+        <v>4.6360029152158137E-2</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>48</v>
@@ -1298,8 +1322,11 @@
         <v>66</v>
       </c>
       <c r="K12" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N12)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>2.4103050418839981E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N12)/N12</f>
+        <v>2.4698356142197841E-2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>116</v>
       </c>
       <c r="N12">
         <v>246.98</v>
@@ -1319,8 +1346,8 @@
         <v>69</v>
       </c>
       <c r="E13" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-224.91)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>4.0404471371277409E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N13)/N13</f>
+        <v>4.2105731181361426E-2</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>48</v>
@@ -1338,8 +1365,12 @@
         <v>72</v>
       </c>
       <c r="K13" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N13)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>8.1587651598676925E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N13)/N13</f>
+        <v>8.8835534213685424E-2</v>
+      </c>
+      <c r="M13" s="3">
+        <f>AVERAGE(E13:E20)</f>
+        <v>7.3456662000961973E-2</v>
       </c>
       <c r="N13">
         <v>224.91</v>
@@ -1359,8 +1390,8 @@
         <v>74</v>
       </c>
       <c r="E14" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-224.83)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>6.2075007300488066E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N14)/N14</f>
+        <v>6.6183338522439156E-2</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>48</v>
@@ -1378,8 +1409,8 @@
         <v>77</v>
       </c>
       <c r="K14" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N14)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>8.4978226364413309E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N14)/N14</f>
+        <v>9.2870168571809783E-2</v>
       </c>
       <c r="N14">
         <v>224.83</v>
@@ -1399,8 +1430,8 @@
         <v>79</v>
       </c>
       <c r="E15" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-225.12)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>0.11265273945605039</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N15)/N15</f>
+        <v>0.12695451314854292</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>48</v>
@@ -1418,8 +1449,8 @@
         <v>82</v>
       </c>
       <c r="K15" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N15)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>8.4766434931089138E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N15)/N15</f>
+        <v>9.2617270788912548E-2</v>
       </c>
       <c r="N15">
         <v>225.12</v>
@@ -1439,8 +1470,8 @@
         <v>84</v>
       </c>
       <c r="E16" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-224.83)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>0.11848657126053715</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N16)/N16</f>
+        <v>0.13441266734866342</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>48</v>
@@ -1458,8 +1489,8 @@
         <v>87</v>
       </c>
       <c r="K16" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N16)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>8.6873527739419976E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N16)/N16</f>
+        <v>9.513854912600625E-2</v>
       </c>
       <c r="N16">
         <v>224.83</v>
@@ -1479,8 +1510,8 @@
         <v>90</v>
       </c>
       <c r="E17" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-238.57)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>-1.3638681169272516E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N17)/N17</f>
+        <v>-1.3455170390241772E-2</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>48</v>
@@ -1498,8 +1529,8 @@
         <v>92</v>
       </c>
       <c r="K17" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N17)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>-2.2282212795132143E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N17)/N17</f>
+        <v>-2.1796537703818539E-2</v>
       </c>
       <c r="N17">
         <v>238.57</v>
@@ -1519,8 +1550,8 @@
         <v>94</v>
       </c>
       <c r="E18" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-230.36)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>3.8002171552660127E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N18)/N18</f>
+        <v>3.9503386004514647E-2</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>48</v>
@@ -1538,8 +1569,8 @@
         <v>30</v>
       </c>
       <c r="K18" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N18)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>2.1576622494053618E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N18)/N18</f>
+        <v>2.2052439659663067E-2</v>
       </c>
       <c r="N18">
         <v>230.36</v>
@@ -1559,8 +1590,8 @@
         <v>98</v>
       </c>
       <c r="E19" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-233.6)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>7.8464633713361528E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N19)/N19</f>
+        <v>8.5145547945205541E-2</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1578,8 +1609,8 @@
         <v>101</v>
       </c>
       <c r="K19" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N19)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>8.6152017994313174E-3</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N19)/N19</f>
+        <v>8.6900684931506909E-3</v>
       </c>
       <c r="N19">
         <v>233.6</v>
@@ -1599,8 +1630,8 @@
         <v>103</v>
       </c>
       <c r="E20" s="2">
-        <f>(Lower_bounds[[#This Row],[Column3]]-230.33)/Lower_bounds[[#This Row],[Column3]]</f>
-        <v>9.6497077629153077E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column3]]-N20)/N20</f>
+        <v>0.10680328224721049</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>48</v>
@@ -1618,8 +1649,8 @@
         <v>106</v>
       </c>
       <c r="K20" s="2">
-        <f>(Lower_bounds[[#This Row],[Column7]]-N20)/Lower_bounds[[#This Row],[Column7]]</f>
-        <v>4.0131688614769109E-2</v>
+        <f>(Lower_bounds[[#This Row],[Column7]]-N20)/N20</f>
+        <v>4.1809577562627515E-2</v>
       </c>
       <c r="N20">
         <v>230.33</v>

</xml_diff>